<commit_message>
Backlog com informações Atualizadas
</commit_message>
<xml_diff>
--- a/private/Documentacao/Backlog.xlsx
+++ b/private/Documentacao/Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro Sousa\Downloads\Celeste\private\Documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9E1E4B-4340-4297-833D-F1EDAC520581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721436D8-2294-4F6E-B4B7-7F8614E760C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{F3F13A2E-DF68-4EFE-B551-2C7EE1D017EE}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="13710" xr2:uid="{F3F13A2E-DF68-4EFE-B551-2C7EE1D017EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
   <si>
     <t>Requisito</t>
   </si>
@@ -185,12 +185,15 @@
   <si>
     <t>Montar diagrama de Solução e Técnico do Projeto.</t>
   </si>
+  <si>
+    <t>Sim</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,6 +267,13 @@
     <font>
       <sz val="12"/>
       <color theme="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -383,31 +393,31 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -448,20 +458,23 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="pt-BR"/>
+              <a:rPr lang="pt-BR" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
               <a:t>Burndown</a:t>
             </a:r>
           </a:p>
@@ -480,16 +493,13 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="pt-BR"/>
@@ -634,7 +644,7 @@
                   <c:v>186</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>186</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>186</c:v>
@@ -751,7 +761,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Backlog!$L$2</c15:sqref>
@@ -777,7 +787,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Backlog!$H$3:$H$6</c15:sqref>
@@ -804,7 +814,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Backlog!$L$3:$L$6</c15:sqref>
@@ -818,7 +828,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-5DF8-42A4-8614-19D27E7E0EEB}"/>
                   </c:ext>
@@ -857,16 +867,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="pt-BR"/>
@@ -916,16 +923,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="800" b="0" i="1" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="pt-BR"/>
@@ -958,16 +962,13 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="800" b="0" i="1" u="sng" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="pt-BR"/>
@@ -1927,8 +1928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{152D3106-CDCB-49CA-A349-14A127939812}">
   <dimension ref="A1:L341"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1979,19 +1980,19 @@
         <v>1</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="11" t="s">
         <v>5</v>
       </c>
       <c r="I2" s="15" t="s">
         <v>37</v>
       </c>
       <c r="J2" s="15"/>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="L2" s="14"/>
+      <c r="L2" s="16"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -2010,16 +2011,16 @@
         <v>1</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="17">
+        <v>41</v>
+      </c>
+      <c r="H3" s="12">
         <v>1</v>
       </c>
-      <c r="I3" s="12">
+      <c r="I3" s="14">
         <f>186</f>
         <v>186</v>
       </c>
-      <c r="J3" s="12"/>
+      <c r="J3" s="14"/>
       <c r="K3" s="13">
         <f>186</f>
         <v>186</v>
@@ -2043,18 +2044,19 @@
         <v>1</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="17">
+        <v>41</v>
+      </c>
+      <c r="H4" s="12">
         <v>2</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="14">
         <f>186-3-5-5-8-13</f>
         <v>152</v>
       </c>
-      <c r="J4" s="12"/>
+      <c r="J4" s="14"/>
       <c r="K4" s="13">
-        <v>186</v>
+        <f>186-3-5-5</f>
+        <v>173</v>
       </c>
       <c r="L4" s="13"/>
     </row>
@@ -2077,14 +2079,14 @@
       <c r="F5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="17">
+      <c r="H5" s="12">
         <v>3</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="14">
         <f>152-13-13-21-13</f>
         <v>92</v>
       </c>
-      <c r="J5" s="12"/>
+      <c r="J5" s="14"/>
       <c r="K5" s="13">
         <v>186</v>
       </c>
@@ -2109,14 +2111,14 @@
       <c r="F6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="17">
+      <c r="H6" s="12">
         <v>4</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="17">
         <f>92-92</f>
         <v>0</v>
       </c>
-      <c r="J6" s="19"/>
+      <c r="J6" s="18"/>
       <c r="K6" s="13">
         <v>186</v>
       </c>
@@ -2141,16 +2143,16 @@
       <c r="F7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="19">
         <f>SUM(D2:D100)</f>
         <v>186</v>
       </c>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
@@ -4922,6 +4924,8 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="I6:J6"/>
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="I5:J5"/>
@@ -4931,8 +4935,6 @@
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="I6:J6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>